<commit_message>
Nueva version de la estructura
</commit_message>
<xml_diff>
--- a/Trunk/Proyecto/Gestion de configuracion/ISW_rep_est_items_config_00_20190904.xlsx
+++ b/Trunk/Proyecto/Gestion de configuracion/ISW_rep_est_items_config_00_20190904.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxiy\Documents\Repositorio\grupo5_4k3_Ing-Software2019\Trunk\Proyecto\Gestion de configuracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myacuzzi\Documents\Personal\FACULTAD\ISW\grupo5_4k3_Ing-Software2019\Trunk\Proyecto\Gestion de configuracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
   <si>
     <t xml:space="preserve">Nombre del Ítem de Configuración </t>
   </si>
@@ -65,42 +65,15 @@
     <t>Planilla de métricas del Sprint</t>
   </si>
   <si>
-    <t>DE_&lt;NroSprint&gt;_&lt;NombreMetrica&gt;.docx</t>
-  </si>
-  <si>
-    <t>http://&lt;NumIPServidor&gt;/DE/Proyecto/Sprint/Sprint#/Métricas del Sprint</t>
-  </si>
-  <si>
     <t>Planilla de métricas del Proyecto</t>
   </si>
   <si>
-    <t>DE_MetricaProyecto_&lt;NombreMetrica&gt;.docx</t>
-  </si>
-  <si>
-    <t>http://&lt;NumIPServidor&gt;/DE/Proyecto/Métricas del Proyecto</t>
-  </si>
-  <si>
     <t>Proyecto</t>
   </si>
   <si>
     <t>User Story</t>
   </si>
   <si>
-    <t>DE_UserStory_&lt;NombreUS&gt;.docx</t>
-  </si>
-  <si>
-    <t>http://&lt;NumIPServidor&gt;/DE/Proyecto/Product Backlog/User Stories</t>
-  </si>
-  <si>
-    <t>Documento de Revisión</t>
-  </si>
-  <si>
-    <t>DE_&lt;NroSprint&gt;_Revision.docx</t>
-  </si>
-  <si>
-    <t>http://&lt;NumIPServidor&gt;/DE/Proyecto/Sprint/Sprint#/Revisiones del Sprint</t>
-  </si>
-  <si>
     <t>Documento de Arquitectura</t>
   </si>
   <si>
@@ -110,15 +83,6 @@
     <t>http://&lt;NumIPServidor&gt;/DE/Producto/Arquitectura del Producto</t>
   </si>
   <si>
-    <t>Código Fuente</t>
-  </si>
-  <si>
-    <t>DE_&lt;NombreClase&gt;.&lt;extensiòn&gt;</t>
-  </si>
-  <si>
-    <t>http://&lt;NumIPServidor&gt;/DE/Producto/Código Fuente</t>
-  </si>
-  <si>
     <t>Lista de Impedimentos</t>
   </si>
   <si>
@@ -134,12 +98,6 @@
     <t>DE_PlanRiesgos.xlsx</t>
   </si>
   <si>
-    <t>Librería</t>
-  </si>
-  <si>
-    <t>DE_&lt;NombreLibreria&gt;.&lt;extensiòn&gt;</t>
-  </si>
-  <si>
     <t>http://&lt;NumIPServidor&gt;/DE/Producto</t>
   </si>
   <si>
@@ -192,13 +150,142 @@
   </si>
   <si>
     <t>http://&lt;NumIPServidor&gt;/ISW/Truck/Proyecto/Requerimientos/User Stories</t>
+  </si>
+  <si>
+    <t>Documento de Linea base</t>
+  </si>
+  <si>
+    <t>ISW_DOC_L_BASE_&lt;ITERxx&gt;_&lt;NOMBRE_LB&gt;_&lt;NN&gt;.docx</t>
+  </si>
+  <si>
+    <t>ISW_MetricaProyecto_&lt;NombreMetrica&gt;.docx</t>
+  </si>
+  <si>
+    <t>http://&lt;NumIPServidor&gt;/ISW/Truck/Proyecto/Métricas del Proyecto</t>
+  </si>
+  <si>
+    <t>ISW_&lt;NroSprint&gt;_&lt;NombreMetrica&gt;.docx</t>
+  </si>
+  <si>
+    <t>http://&lt;NumIPServidor&gt;/ISW/Truck/Proyecto/Sprint/Sprint#/Métricas</t>
+  </si>
+  <si>
+    <t>Codigo fuente del Sprint</t>
+  </si>
+  <si>
+    <t>http://&lt;NumIPServidor&gt;/ISW/Truck/Proyecto/Sprint/Sprint#/Codigo fuente</t>
+  </si>
+  <si>
+    <t>http://&lt;NumIPServidor&gt;/ISW/Truck/Proyecto/Sprint/Sprint#/Revisiones</t>
+  </si>
+  <si>
+    <t>ISW_&lt;NroSprint&gt;_Revision.docx</t>
+  </si>
+  <si>
+    <t>Documento de Revisión del Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documento de bibliografia </t>
+  </si>
+  <si>
+    <t>ISW_&lt;NOMBRE_DOCUMENTO&gt;.pdf</t>
+  </si>
+  <si>
+    <t>http://&lt;NumIPServidor&gt;/ISW/TP_Evaluables/Bibliografia</t>
+  </si>
+  <si>
+    <t>Trabajos teoricos</t>
+  </si>
+  <si>
+    <t>http://&lt;NumIPServidor&gt;/ISW/TP_Evaluables/Teoricos</t>
+  </si>
+  <si>
+    <t>ISW_&lt;NOMBRE_TRABAJO&gt;.pdf</t>
+  </si>
+  <si>
+    <t>Trabajos practicos</t>
+  </si>
+  <si>
+    <t>http://&lt;NumIPServidor&gt;/ISW/TP_Evaluables/Practicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigla </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significado </t>
+  </si>
+  <si>
+    <t>&lt;NumIPServidor&gt;</t>
+  </si>
+  <si>
+    <t>Número de IP del servidor en el que se encuentra el repositorio del Proyecto.</t>
+  </si>
+  <si>
+    <t>&lt;NroSprint&gt;</t>
+  </si>
+  <si>
+    <t>Número del Sprint que se encuentra en curso.</t>
+  </si>
+  <si>
+    <t>&lt;NombreUS&gt;</t>
+  </si>
+  <si>
+    <t>Nombre que se le asigna a la User Story.</t>
+  </si>
+  <si>
+    <t>&lt;NombreMetrica&gt;</t>
+  </si>
+  <si>
+    <t>Nombre por el cual se la identifica a la métrica.</t>
+  </si>
+  <si>
+    <t>Nombre que identifica a cada clase implementada.</t>
+  </si>
+  <si>
+    <t>&lt;NOMBRE_LIBRERIA&gt;</t>
+  </si>
+  <si>
+    <t>Nombre de la librería.</t>
+  </si>
+  <si>
+    <t>&lt;extensión&gt;</t>
+  </si>
+  <si>
+    <t>Nombre de la extensiòn de un archivo identificado como ítem de configuración.</t>
+  </si>
+  <si>
+    <t>&lt;NOMBRE_COMPONENTE_SW&gt;</t>
+  </si>
+  <si>
+    <t>&lt;NOMBRE_DOCUMENTO&gt;</t>
+  </si>
+  <si>
+    <t>Nombre del documento dibliografico.</t>
+  </si>
+  <si>
+    <t>&lt;ITERxx&gt;</t>
+  </si>
+  <si>
+    <t>&lt;NN&gt;</t>
+  </si>
+  <si>
+    <t>&lt;YYYYMMDD&gt;</t>
+  </si>
+  <si>
+    <t>Numero de iteracion del proyecto</t>
+  </si>
+  <si>
+    <t>Numero cardinal empezando de 00.</t>
+  </si>
+  <si>
+    <t>Fecha en formato numerico.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,11 +307,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -241,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -260,11 +353,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -282,8 +399,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -609,21 +743,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:F21"/>
+  <dimension ref="C2:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.453125" customWidth="1"/>
-    <col min="3" max="3" width="30.6328125" customWidth="1"/>
-    <col min="4" max="4" width="44.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="64.453125" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -637,7 +771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -651,7 +785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
@@ -665,218 +799,390 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
+    <row r="5" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="F20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="F25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="F26" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>